<commit_message>
[#84422868] allowing spaces in xlsx
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/manual_measurements.xlsx
+++ b/spec/fixtures/files/manual_measurements.xlsx
@@ -397,12 +397,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -410,11 +410,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -450,7 +450,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -462,23 +462,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -490,11 +486,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -516,10 +512,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
   </cellXfs>
@@ -595,14 +587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="A1:AI50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG26" activeCellId="0" sqref="AG26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U2" activeCellId="0" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="14" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -960,7 +952,7 @@
     </row>
     <row r="6" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9"/>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="6" t="n">
@@ -1170,7 +1162,7 @@
     </row>
     <row r="8" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="6" t="n">
@@ -1380,7 +1372,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="6" t="n">
@@ -1476,7 +1468,7 @@
       <c r="AG10" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="AH10" s="17" t="s">
+      <c r="AH10" s="16" t="s">
         <v>24</v>
       </c>
       <c r="AI10" s="7" t="s">
@@ -1590,7 +1582,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9"/>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="6" t="n">
@@ -1689,7 +1681,7 @@
       <c r="AH12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AI12" s="17" t="s">
+      <c r="AI12" s="16" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1800,7 +1792,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9"/>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="7" t="s">
@@ -1904,44 +1896,44 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19"/>
-      <c r="O15" s="19"/>
-      <c r="P15" s="19"/>
-      <c r="Q15" s="19"/>
-      <c r="R15" s="19"/>
-      <c r="S15" s="19"/>
-      <c r="T15" s="19"/>
-      <c r="U15" s="19"/>
-      <c r="V15" s="19"/>
-      <c r="W15" s="19"/>
-      <c r="X15" s="19"/>
-      <c r="Y15" s="19"/>
-      <c r="Z15" s="19"/>
-      <c r="AA15" s="19"/>
-      <c r="AB15" s="19"/>
-      <c r="AC15" s="19"/>
-      <c r="AD15" s="19"/>
-      <c r="AE15" s="19"/>
-      <c r="AF15" s="19"/>
-      <c r="AG15" s="19"/>
-      <c r="AH15" s="19"/>
-      <c r="AI15" s="20"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="18"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="18"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="19"/>
     </row>
     <row r="16" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="20" t="s">
         <v>33</v>
       </c>
       <c r="B16" s="11"/>
@@ -2046,8 +2038,8 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="21"/>
-      <c r="B17" s="16" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C17" s="6" t="n">
@@ -2151,7 +2143,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="21"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="13" t="s">
         <v>19</v>
       </c>
@@ -2256,8 +2248,8 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="21"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="6" t="n">
@@ -2353,7 +2345,7 @@
       <c r="AG19" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="AH19" s="17" t="s">
+      <c r="AH19" s="16" t="s">
         <v>37</v>
       </c>
       <c r="AI19" s="7" t="s">
@@ -2361,7 +2353,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="21"/>
+      <c r="A20" s="20"/>
       <c r="B20" s="13" t="s">
         <v>25</v>
       </c>
@@ -2466,8 +2458,8 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="21"/>
-      <c r="B21" s="16" t="s">
+      <c r="A21" s="20"/>
+      <c r="B21" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="7" t="s">
@@ -2571,7 +2563,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="21"/>
+      <c r="A22" s="20"/>
       <c r="B22" s="13" t="s">
         <v>39</v>
       </c>
@@ -2668,7 +2660,7 @@
       <c r="AG22" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="AH22" s="22" t="s">
+      <c r="AH22" s="21" t="s">
         <v>40</v>
       </c>
       <c r="AI22" s="15" t="s">
@@ -2676,44 +2668,44 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="19"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19"/>
-      <c r="O23" s="19"/>
-      <c r="P23" s="19"/>
-      <c r="Q23" s="19"/>
-      <c r="R23" s="19"/>
-      <c r="S23" s="19"/>
-      <c r="T23" s="19"/>
-      <c r="U23" s="19"/>
-      <c r="V23" s="19"/>
-      <c r="W23" s="19"/>
-      <c r="X23" s="19"/>
-      <c r="Y23" s="19"/>
-      <c r="Z23" s="19"/>
-      <c r="AA23" s="19"/>
-      <c r="AB23" s="19"/>
-      <c r="AC23" s="19"/>
-      <c r="AD23" s="19"/>
-      <c r="AE23" s="19"/>
-      <c r="AF23" s="19"/>
-      <c r="AG23" s="19"/>
-      <c r="AH23" s="23"/>
-      <c r="AI23" s="24"/>
+      <c r="A23" s="17"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="18"/>
+      <c r="V23" s="18"/>
+      <c r="W23" s="18"/>
+      <c r="X23" s="18"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+      <c r="AA23" s="18"/>
+      <c r="AB23" s="18"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="18"/>
+      <c r="AE23" s="18"/>
+      <c r="AF23" s="18"/>
+      <c r="AG23" s="18"/>
+      <c r="AH23" s="22"/>
+      <c r="AI23" s="23"/>
     </row>
     <row r="24" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="11"/>
@@ -2818,7 +2810,7 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="25"/>
+      <c r="A25" s="24"/>
       <c r="B25" s="13" t="s">
         <v>42</v>
       </c>
@@ -2923,8 +2915,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="25"/>
-      <c r="B26" s="16" t="s">
+      <c r="A26" s="24"/>
+      <c r="B26" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="6"/>
@@ -2976,7 +2968,7 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="25"/>
+      <c r="A27" s="24"/>
       <c r="B27" s="13" t="s">
         <v>23</v>
       </c>
@@ -3073,16 +3065,16 @@
       <c r="AG27" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="AH27" s="22" t="s">
+      <c r="AH27" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AI27" s="22" t="s">
+      <c r="AI27" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="25"/>
-      <c r="B28" s="16" t="s">
+      <c r="A28" s="24"/>
+      <c r="B28" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="6" t="n">
@@ -3178,15 +3170,15 @@
       <c r="AG28" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="AH28" s="17" t="s">
+      <c r="AH28" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AI28" s="17" t="s">
+      <c r="AI28" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="25"/>
+      <c r="A29" s="24"/>
       <c r="B29" s="13" t="s">
         <v>47</v>
       </c>
@@ -3291,8 +3283,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="25"/>
-      <c r="B30" s="16" t="s">
+      <c r="A30" s="24"/>
+      <c r="B30" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C30" s="6" t="n">
@@ -3388,15 +3380,15 @@
       <c r="AG30" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="AH30" s="17" t="s">
+      <c r="AH30" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AI30" s="17" t="s">
+      <c r="AI30" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="25"/>
+      <c r="A31" s="24"/>
       <c r="B31" s="13" t="s">
         <v>30</v>
       </c>
@@ -3501,8 +3493,8 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="25"/>
-      <c r="B32" s="16" t="s">
+      <c r="A32" s="24"/>
+      <c r="B32" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="6" t="n">
@@ -3598,15 +3590,15 @@
       <c r="AG32" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="AH32" s="17" t="s">
+      <c r="AH32" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="AI32" s="17" t="s">
+      <c r="AI32" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="25"/>
+      <c r="A33" s="24"/>
       <c r="B33" s="13" t="s">
         <v>31</v>
       </c>
@@ -3711,44 +3703,44 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18"/>
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-      <c r="O34" s="19"/>
-      <c r="P34" s="19"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="19"/>
-      <c r="S34" s="19"/>
-      <c r="T34" s="19"/>
-      <c r="U34" s="19"/>
-      <c r="V34" s="19"/>
-      <c r="W34" s="19"/>
-      <c r="X34" s="19"/>
-      <c r="Y34" s="19"/>
-      <c r="Z34" s="19"/>
-      <c r="AA34" s="19"/>
-      <c r="AB34" s="19"/>
-      <c r="AC34" s="19"/>
-      <c r="AD34" s="19"/>
-      <c r="AE34" s="19"/>
-      <c r="AF34" s="19"/>
-      <c r="AG34" s="19"/>
-      <c r="AH34" s="23"/>
-      <c r="AI34" s="24"/>
+      <c r="A34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="18"/>
+      <c r="O34" s="18"/>
+      <c r="P34" s="18"/>
+      <c r="Q34" s="18"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="18"/>
+      <c r="U34" s="18"/>
+      <c r="V34" s="18"/>
+      <c r="W34" s="18"/>
+      <c r="X34" s="18"/>
+      <c r="Y34" s="18"/>
+      <c r="Z34" s="18"/>
+      <c r="AA34" s="18"/>
+      <c r="AB34" s="18"/>
+      <c r="AC34" s="18"/>
+      <c r="AD34" s="18"/>
+      <c r="AE34" s="18"/>
+      <c r="AF34" s="18"/>
+      <c r="AG34" s="18"/>
+      <c r="AH34" s="22"/>
+      <c r="AI34" s="23"/>
     </row>
     <row r="35" customFormat="false" ht="14" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="26" t="s">
+      <c r="A35" s="25" t="s">
         <v>53</v>
       </c>
       <c r="B35" s="11"/>
@@ -3853,7 +3845,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="26"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="13" t="s">
         <v>42</v>
       </c>
@@ -3958,8 +3950,8 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="26"/>
-      <c r="B37" s="16" t="s">
+      <c r="A37" s="25"/>
+      <c r="B37" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C37" s="6" t="n">
@@ -4063,7 +4055,7 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="26"/>
+      <c r="A38" s="25"/>
       <c r="B38" s="13" t="s">
         <v>23</v>
       </c>
@@ -4160,16 +4152,16 @@
       <c r="AG38" s="14" t="n">
         <v>5</v>
       </c>
-      <c r="AH38" s="22" t="s">
+      <c r="AH38" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AI38" s="22" t="s">
+      <c r="AI38" s="21" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="26"/>
-      <c r="B39" s="16" t="s">
+      <c r="A39" s="25"/>
+      <c r="B39" s="5" t="s">
         <v>34</v>
       </c>
       <c r="C39" s="6" t="n">
@@ -4265,15 +4257,15 @@
       <c r="AG39" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="AH39" s="17" t="s">
+      <c r="AH39" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="AI39" s="17" t="s">
+      <c r="AI39" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="26"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="13" t="s">
         <v>47</v>
       </c>
@@ -4378,8 +4370,8 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="26"/>
-      <c r="B41" s="16" t="s">
+      <c r="A41" s="25"/>
+      <c r="B41" s="5" t="s">
         <v>49</v>
       </c>
       <c r="C41" s="6" t="n">
@@ -4475,15 +4467,15 @@
       <c r="AG41" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="AH41" s="17" t="s">
+      <c r="AH41" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="AI41" s="17" t="s">
+      <c r="AI41" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="26"/>
+      <c r="A42" s="25"/>
       <c r="B42" s="13" t="s">
         <v>30</v>
       </c>
@@ -4588,8 +4580,8 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="26"/>
-      <c r="B43" s="16" t="s">
+      <c r="A43" s="25"/>
+      <c r="B43" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C43" s="6" t="n">
@@ -4685,15 +4677,15 @@
       <c r="AG43" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="AH43" s="17" t="s">
+      <c r="AH43" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="AI43" s="17" t="s">
+      <c r="AI43" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="26"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="13" t="s">
         <v>31</v>
       </c>
@@ -4798,118 +4790,98 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="18"/>
-      <c r="B45" s="19"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="19"/>
-      <c r="E45" s="19"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="19"/>
-      <c r="H45" s="19"/>
-      <c r="I45" s="19"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
-      <c r="L45" s="19"/>
-      <c r="M45" s="19"/>
-      <c r="N45" s="19"/>
-      <c r="O45" s="19"/>
-      <c r="P45" s="19"/>
-      <c r="Q45" s="19"/>
-      <c r="R45" s="19"/>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="19"/>
-      <c r="Z45" s="19"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="19"/>
-      <c r="AD45" s="19"/>
-      <c r="AE45" s="19"/>
-      <c r="AF45" s="19"/>
-      <c r="AG45" s="19"/>
-      <c r="AH45" s="19"/>
-      <c r="AI45" s="20"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="18"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="18"/>
+      <c r="N45" s="18"/>
+      <c r="O45" s="18"/>
+      <c r="P45" s="18"/>
+      <c r="Q45" s="18"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="18"/>
+      <c r="U45" s="18"/>
+      <c r="V45" s="18"/>
+      <c r="W45" s="18"/>
+      <c r="X45" s="18"/>
+      <c r="Y45" s="18"/>
+      <c r="Z45" s="18"/>
+      <c r="AA45" s="18"/>
+      <c r="AB45" s="18"/>
+      <c r="AC45" s="18"/>
+      <c r="AD45" s="18"/>
+      <c r="AE45" s="18"/>
+      <c r="AF45" s="18"/>
+      <c r="AG45" s="18"/>
+      <c r="AH45" s="18"/>
+      <c r="AI45" s="19"/>
     </row>
     <row r="46" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="28"/>
-      <c r="J46" s="28"/>
-      <c r="K46" s="28"/>
-      <c r="L46" s="28"/>
-      <c r="M46" s="28"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="28"/>
-      <c r="P46" s="28"/>
-      <c r="Q46" s="28"/>
-      <c r="R46" s="28"/>
-      <c r="S46" s="28"/>
-      <c r="T46" s="28"/>
-      <c r="U46" s="28"/>
-      <c r="V46" s="28"/>
-      <c r="W46" s="28"/>
-      <c r="X46" s="28"/>
-      <c r="Y46" s="28"/>
-      <c r="Z46" s="28"/>
-      <c r="AA46" s="28"/>
-      <c r="AB46" s="28"/>
-      <c r="AC46" s="28"/>
-      <c r="AD46" s="28"/>
-      <c r="AE46" s="28"/>
-      <c r="AF46" s="28"/>
-      <c r="AG46" s="28"/>
-      <c r="AH46" s="28"/>
-      <c r="AI46" s="28"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="27"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="27"/>
+      <c r="M46" s="27"/>
+      <c r="N46" s="27"/>
+      <c r="O46" s="27"/>
+      <c r="P46" s="27"/>
+      <c r="Q46" s="27"/>
+      <c r="R46" s="27"/>
+      <c r="S46" s="27"/>
+      <c r="T46" s="27"/>
+      <c r="U46" s="27"/>
+      <c r="V46" s="27"/>
+      <c r="W46" s="27"/>
+      <c r="X46" s="27"/>
+      <c r="Y46" s="27"/>
+      <c r="Z46" s="27"/>
+      <c r="AA46" s="27"/>
+      <c r="AB46" s="27"/>
+      <c r="AC46" s="27"/>
+      <c r="AD46" s="27"/>
+      <c r="AE46" s="27"/>
+      <c r="AF46" s="27"/>
+      <c r="AG46" s="27"/>
+      <c r="AH46" s="27"/>
+      <c r="AI46" s="27"/>
     </row>
     <row r="50" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="C50" s="29"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29"/>
-      <c r="F50" s="29"/>
-      <c r="G50" s="29"/>
-      <c r="H50" s="29"/>
-      <c r="I50" s="29"/>
-      <c r="J50" s="29"/>
-      <c r="K50" s="29"/>
-      <c r="L50" s="29"/>
-      <c r="M50" s="29"/>
-      <c r="N50" s="29"/>
-      <c r="O50" s="29"/>
-      <c r="P50" s="30"/>
-      <c r="Q50" s="30"/>
-      <c r="R50" s="30"/>
-      <c r="S50" s="30"/>
-      <c r="T50" s="30"/>
-      <c r="U50" s="30"/>
-      <c r="V50" s="30"/>
-      <c r="W50" s="30"/>
-      <c r="X50" s="30"/>
-      <c r="Y50" s="30"/>
-      <c r="Z50" s="30"/>
-      <c r="AA50" s="30"/>
-      <c r="AB50" s="30"/>
-      <c r="AC50" s="30"/>
-      <c r="AD50" s="30"/>
-      <c r="AE50" s="30"/>
-      <c r="AF50" s="30"/>
-      <c r="AG50" s="30"/>
-      <c r="AH50" s="30"/>
-      <c r="AI50" s="30"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
+      <c r="L50" s="28"/>
+      <c r="M50" s="28"/>
+      <c r="N50" s="28"/>
+      <c r="O50" s="28"/>
     </row>
   </sheetData>
   <sheetProtection sheet="true" objects="true" scenarios="true"/>
@@ -4933,8 +4905,8 @@
     <mergeCell ref="B50:O50"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>